<commit_message>
Add zombies to level and zombie health
</commit_message>
<xml_diff>
--- a/LevelDesign_excel/Level3.xlsx
+++ b/LevelDesign_excel/Level3.xlsx
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U39" sqref="U39:V41"/>
+    <sheetView tabSelected="1" topLeftCell="L22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AU46" sqref="AU46:AU47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed typing name bug
Add ai and traps in level3 and renew highscore
</commit_message>
<xml_diff>
--- a/LevelDesign_excel/Level3.xlsx
+++ b/LevelDesign_excel/Level3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shing\Desktop\SP3_Grp3\LevelDesign_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\SP3_Grp3\LevelDesign_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -553,21 +553,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BU26" sqref="BU26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y47" sqref="Y47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="19" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="44" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="50" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="15" width="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="48" width="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="3" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="2.7109375" bestFit="1" customWidth="1"/>
@@ -1535,8 +1537,8 @@
       <c r="B7" s="13">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" s="19">
+        <v>33</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1941,8 +1943,8 @@
       <c r="AF9">
         <v>0</v>
       </c>
-      <c r="AG9">
-        <v>0</v>
+      <c r="AG9" s="2">
+        <v>30</v>
       </c>
       <c r="AH9">
         <v>0</v>
@@ -1953,8 +1955,8 @@
       <c r="AJ9">
         <v>0</v>
       </c>
-      <c r="AK9">
-        <v>0</v>
+      <c r="AK9" s="9">
+        <v>14</v>
       </c>
       <c r="AL9">
         <v>0</v>
@@ -2036,8 +2038,8 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10">
-        <v>0</v>
+      <c r="L10" s="2">
+        <v>30</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -2075,8 +2077,8 @@
       <c r="X10">
         <v>0</v>
       </c>
-      <c r="Y10">
-        <v>0</v>
+      <c r="Y10" s="2">
+        <v>30</v>
       </c>
       <c r="Z10">
         <v>0</v>
@@ -2090,8 +2092,8 @@
       <c r="AC10">
         <v>0</v>
       </c>
-      <c r="AD10">
-        <v>0</v>
+      <c r="AD10" s="9">
+        <v>14</v>
       </c>
       <c r="AE10">
         <v>0</v>
@@ -2138,8 +2140,8 @@
       <c r="AS10">
         <v>0</v>
       </c>
-      <c r="AT10">
-        <v>0</v>
+      <c r="AT10" s="9">
+        <v>14</v>
       </c>
       <c r="AU10">
         <v>0</v>
@@ -2364,8 +2366,8 @@
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="R12">
-        <v>0</v>
+      <c r="R12" s="17">
+        <v>32</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -2376,8 +2378,8 @@
       <c r="U12">
         <v>0</v>
       </c>
-      <c r="V12">
-        <v>0</v>
+      <c r="V12" s="9">
+        <v>14</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -2412,8 +2414,8 @@
       <c r="AG12">
         <v>0</v>
       </c>
-      <c r="AH12">
-        <v>0</v>
+      <c r="AH12" s="9">
+        <v>14</v>
       </c>
       <c r="AI12">
         <v>0</v>
@@ -2483,8 +2485,8 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13">
-        <v>0</v>
+      <c r="E13" s="2">
+        <v>30</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -2495,8 +2497,8 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
-        <v>0</v>
+      <c r="I13" s="2">
+        <v>30</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2582,14 +2584,14 @@
       <c r="AK13">
         <v>0</v>
       </c>
-      <c r="AL13">
-        <v>0</v>
+      <c r="AL13" s="9">
+        <v>14</v>
       </c>
       <c r="AM13">
         <v>0</v>
       </c>
-      <c r="AN13">
-        <v>0</v>
+      <c r="AN13" s="9">
+        <v>14</v>
       </c>
       <c r="AO13">
         <v>0</v>
@@ -2710,8 +2712,8 @@
       <c r="AA14">
         <v>0</v>
       </c>
-      <c r="AB14">
-        <v>0</v>
+      <c r="AB14" s="18">
+        <v>31</v>
       </c>
       <c r="AC14">
         <v>0</v>
@@ -2761,8 +2763,8 @@
       <c r="AR14">
         <v>0</v>
       </c>
-      <c r="AS14">
-        <v>0</v>
+      <c r="AS14" s="9">
+        <v>14</v>
       </c>
       <c r="AT14">
         <v>0</v>
@@ -2871,8 +2873,8 @@
       <c r="AB15">
         <v>0</v>
       </c>
-      <c r="AC15">
-        <v>0</v>
+      <c r="AC15" s="9">
+        <v>14</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -3047,8 +3049,8 @@
       <c r="AH16">
         <v>0</v>
       </c>
-      <c r="AI16">
-        <v>0</v>
+      <c r="AI16" s="9">
+        <v>14</v>
       </c>
       <c r="AJ16">
         <v>0</v>
@@ -3217,8 +3219,8 @@
       <c r="AL17">
         <v>0</v>
       </c>
-      <c r="AM17">
-        <v>0</v>
+      <c r="AM17" s="18">
+        <v>31</v>
       </c>
       <c r="AN17">
         <v>0</v>
@@ -3232,8 +3234,8 @@
       <c r="AQ17">
         <v>0</v>
       </c>
-      <c r="AR17">
-        <v>0</v>
+      <c r="AR17" s="9">
+        <v>14</v>
       </c>
       <c r="AS17">
         <v>0</v>
@@ -3282,8 +3284,8 @@
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18">
-        <v>0</v>
+      <c r="H18" s="2">
+        <v>30</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -3333,8 +3335,8 @@
       <c r="X18">
         <v>0</v>
       </c>
-      <c r="Y18">
-        <v>0</v>
+      <c r="Y18" s="9">
+        <v>14</v>
       </c>
       <c r="Z18">
         <v>0</v>
@@ -3506,8 +3508,8 @@
       <c r="AC19">
         <v>0</v>
       </c>
-      <c r="AD19">
-        <v>0</v>
+      <c r="AD19" s="2">
+        <v>30</v>
       </c>
       <c r="AE19">
         <v>0</v>
@@ -3518,8 +3520,8 @@
       <c r="AG19">
         <v>0</v>
       </c>
-      <c r="AH19">
-        <v>0</v>
+      <c r="AH19" s="9">
+        <v>14</v>
       </c>
       <c r="AI19">
         <v>0</v>
@@ -3539,8 +3541,8 @@
       <c r="AN19">
         <v>0</v>
       </c>
-      <c r="AO19">
-        <v>0</v>
+      <c r="AO19" s="9">
+        <v>14</v>
       </c>
       <c r="AP19">
         <v>0</v>
@@ -3554,8 +3556,8 @@
       <c r="AS19">
         <v>0</v>
       </c>
-      <c r="AT19">
-        <v>0</v>
+      <c r="AT19" s="9">
+        <v>14</v>
       </c>
       <c r="AU19">
         <v>0</v>
@@ -3914,8 +3916,8 @@
       <c r="G22">
         <v>0</v>
       </c>
-      <c r="H22">
-        <v>0</v>
+      <c r="H22" s="5">
+        <v>13</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -3938,8 +3940,8 @@
       <c r="O22" s="13">
         <v>1</v>
       </c>
-      <c r="P22">
-        <v>0</v>
+      <c r="P22" s="8">
+        <v>121</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -4361,8 +4363,8 @@
       <c r="D25" s="13">
         <v>1</v>
       </c>
-      <c r="E25">
-        <v>0</v>
+      <c r="E25" s="14">
+        <v>110</v>
       </c>
       <c r="F25" s="13">
         <v>1</v>
@@ -4555,8 +4557,8 @@
       <c r="R26">
         <v>0</v>
       </c>
-      <c r="S26">
-        <v>0</v>
+      <c r="S26" s="19">
+        <v>33</v>
       </c>
       <c r="T26" s="13">
         <v>1</v>
@@ -4680,8 +4682,8 @@
       <c r="I27">
         <v>0</v>
       </c>
-      <c r="J27">
-        <v>0</v>
+      <c r="J27" s="9">
+        <v>14</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -5142,8 +5144,8 @@
       <c r="K30">
         <v>0</v>
       </c>
-      <c r="L30">
-        <v>0</v>
+      <c r="L30" s="9">
+        <v>14</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -5217,8 +5219,8 @@
       <c r="AJ30">
         <v>0</v>
       </c>
-      <c r="AK30">
-        <v>0</v>
+      <c r="AK30" s="18">
+        <v>31</v>
       </c>
       <c r="AL30">
         <v>0</v>
@@ -5244,8 +5246,8 @@
       <c r="AS30">
         <v>0</v>
       </c>
-      <c r="AT30">
-        <v>0</v>
+      <c r="AT30" s="9">
+        <v>14</v>
       </c>
       <c r="AU30">
         <v>0</v>
@@ -5345,8 +5347,8 @@
       <c r="AB31">
         <v>0</v>
       </c>
-      <c r="AC31">
-        <v>0</v>
+      <c r="AC31" s="18">
+        <v>31</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -5387,14 +5389,14 @@
       <c r="AP31" s="13">
         <v>1</v>
       </c>
-      <c r="AQ31">
-        <v>0</v>
+      <c r="AQ31" s="9">
+        <v>14</v>
       </c>
       <c r="AR31">
         <v>0</v>
       </c>
-      <c r="AS31">
-        <v>0</v>
+      <c r="AS31" s="9">
+        <v>14</v>
       </c>
       <c r="AT31" s="13">
         <v>1</v>
@@ -5548,8 +5550,8 @@
       <c r="AS32">
         <v>0</v>
       </c>
-      <c r="AT32">
-        <v>0</v>
+      <c r="AT32" s="9">
+        <v>14</v>
       </c>
       <c r="AU32">
         <v>0</v>
@@ -5887,8 +5889,8 @@
       <c r="F35">
         <v>0</v>
       </c>
-      <c r="G35">
-        <v>0</v>
+      <c r="G35" s="2">
+        <v>30</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -5935,8 +5937,8 @@
       <c r="V35">
         <v>0</v>
       </c>
-      <c r="W35">
-        <v>0</v>
+      <c r="W35" s="18">
+        <v>31</v>
       </c>
       <c r="X35">
         <v>0</v>
@@ -5971,8 +5973,8 @@
       <c r="AH35" s="13">
         <v>1</v>
       </c>
-      <c r="AI35">
-        <v>0</v>
+      <c r="AI35" s="9">
+        <v>14</v>
       </c>
       <c r="AJ35">
         <v>0</v>
@@ -6129,8 +6131,8 @@
       <c r="AJ36" s="13">
         <v>1</v>
       </c>
-      <c r="AK36">
-        <v>0</v>
+      <c r="AK36" s="9">
+        <v>14</v>
       </c>
       <c r="AL36">
         <v>0</v>
@@ -6147,8 +6149,8 @@
       <c r="AP36">
         <v>0</v>
       </c>
-      <c r="AQ36">
-        <v>0</v>
+      <c r="AQ36" s="18">
+        <v>31</v>
       </c>
       <c r="AR36" s="13">
         <v>1</v>
@@ -6156,8 +6158,8 @@
       <c r="AS36">
         <v>0</v>
       </c>
-      <c r="AT36">
-        <v>0</v>
+      <c r="AT36" s="9">
+        <v>14</v>
       </c>
       <c r="AU36">
         <v>0</v>
@@ -6209,8 +6211,8 @@
       <c r="L37">
         <v>0</v>
       </c>
-      <c r="M37">
-        <v>0</v>
+      <c r="M37" s="2">
+        <v>30</v>
       </c>
       <c r="N37">
         <v>0</v>
@@ -6334,8 +6336,8 @@
       <c r="C38">
         <v>0</v>
       </c>
-      <c r="D38">
-        <v>0</v>
+      <c r="D38" s="2">
+        <v>30</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -7220,17 +7222,17 @@
       <c r="AS43" s="13">
         <v>1</v>
       </c>
-      <c r="AT43" s="13">
-        <v>1</v>
-      </c>
-      <c r="AU43" s="13">
-        <v>1</v>
-      </c>
-      <c r="AV43" s="13">
-        <v>1</v>
-      </c>
-      <c r="AW43" s="13">
-        <v>1</v>
+      <c r="AT43">
+        <v>0</v>
+      </c>
+      <c r="AU43">
+        <v>0</v>
+      </c>
+      <c r="AV43">
+        <v>0</v>
+      </c>
+      <c r="AW43" s="8">
+        <v>120</v>
       </c>
       <c r="AX43" s="13">
         <v>1</v>
@@ -7449,11 +7451,11 @@
       <c r="T45" s="13">
         <v>1</v>
       </c>
-      <c r="U45">
-        <v>0</v>
-      </c>
-      <c r="V45">
-        <v>0</v>
+      <c r="U45" s="14">
+        <v>110</v>
+      </c>
+      <c r="V45" s="14">
+        <v>110</v>
       </c>
       <c r="W45" s="13">
         <v>1</v>
@@ -7547,59 +7549,59 @@
       <c r="B46" s="13">
         <v>1</v>
       </c>
-      <c r="C46" s="13">
-        <v>1</v>
-      </c>
-      <c r="D46" s="13">
-        <v>1</v>
-      </c>
-      <c r="E46" s="13">
-        <v>1</v>
-      </c>
-      <c r="F46" s="13">
-        <v>1</v>
-      </c>
-      <c r="G46" s="13">
-        <v>1</v>
-      </c>
-      <c r="H46" s="13">
-        <v>1</v>
-      </c>
-      <c r="I46" s="13">
-        <v>1</v>
-      </c>
-      <c r="J46" s="13">
-        <v>1</v>
-      </c>
-      <c r="K46" s="13">
-        <v>1</v>
-      </c>
-      <c r="L46" s="13">
-        <v>1</v>
-      </c>
-      <c r="M46" s="13">
-        <v>1</v>
-      </c>
-      <c r="N46" s="13">
-        <v>1</v>
-      </c>
-      <c r="O46" s="13">
-        <v>1</v>
-      </c>
-      <c r="P46" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q46" s="13">
-        <v>1</v>
-      </c>
-      <c r="R46" s="13">
-        <v>1</v>
-      </c>
-      <c r="S46" s="13">
-        <v>1</v>
-      </c>
-      <c r="T46" s="13">
-        <v>1</v>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" s="9">
+        <v>14</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" s="9">
+        <v>14</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46" s="9">
+        <v>14</v>
+      </c>
+      <c r="O46" s="9">
+        <v>14</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="9">
+        <v>14</v>
+      </c>
+      <c r="R46" s="9">
+        <v>14</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
       </c>
       <c r="U46">
         <v>0</v>
@@ -7607,74 +7609,74 @@
       <c r="V46">
         <v>0</v>
       </c>
-      <c r="W46" s="13">
-        <v>1</v>
-      </c>
-      <c r="X46" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y46" s="13">
-        <v>1</v>
-      </c>
-      <c r="Z46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AB46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AC46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AD46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AE46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AF46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AG46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AH46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AI46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AJ46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AK46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AL46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AM46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AN46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AO46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AP46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AQ46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AR46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AS46" s="13">
-        <v>1</v>
+      <c r="W46">
+        <v>0</v>
+      </c>
+      <c r="X46">
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <v>0</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
+      <c r="AA46">
+        <v>0</v>
+      </c>
+      <c r="AB46">
+        <v>0</v>
+      </c>
+      <c r="AC46">
+        <v>0</v>
+      </c>
+      <c r="AD46">
+        <v>0</v>
+      </c>
+      <c r="AE46">
+        <v>0</v>
+      </c>
+      <c r="AF46" s="2">
+        <v>30</v>
+      </c>
+      <c r="AG46">
+        <v>0</v>
+      </c>
+      <c r="AH46">
+        <v>0</v>
+      </c>
+      <c r="AI46">
+        <v>0</v>
+      </c>
+      <c r="AJ46">
+        <v>0</v>
+      </c>
+      <c r="AK46">
+        <v>0</v>
+      </c>
+      <c r="AL46">
+        <v>0</v>
+      </c>
+      <c r="AM46">
+        <v>0</v>
+      </c>
+      <c r="AN46">
+        <v>0</v>
+      </c>
+      <c r="AO46">
+        <v>0</v>
+      </c>
+      <c r="AP46">
+        <v>0</v>
+      </c>
+      <c r="AQ46">
+        <v>0</v>
+      </c>
+      <c r="AR46">
+        <v>0</v>
+      </c>
+      <c r="AS46">
+        <v>0</v>
       </c>
       <c r="AT46">
         <v>0</v>
@@ -7708,8 +7710,8 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
-        <v>0</v>
+      <c r="F47" s="9">
+        <v>14</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -7723,11 +7725,11 @@
       <c r="J47">
         <v>0</v>
       </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
-        <v>0</v>
+      <c r="K47" s="9">
+        <v>14</v>
+      </c>
+      <c r="L47" s="9">
+        <v>14</v>
       </c>
       <c r="M47">
         <v>0</v>
@@ -7765,8 +7767,8 @@
       <c r="X47">
         <v>0</v>
       </c>
-      <c r="Y47">
-        <v>0</v>
+      <c r="Y47" s="18">
+        <v>31</v>
       </c>
       <c r="Z47">
         <v>0</v>
@@ -7834,8 +7836,8 @@
       <c r="AU47">
         <v>0</v>
       </c>
-      <c r="AV47">
-        <v>0</v>
+      <c r="AV47" s="17">
+        <v>32</v>
       </c>
       <c r="AW47">
         <v>0</v>

</xml_diff>

<commit_message>
Finished Level3 change zombies range and speed
</commit_message>
<xml_diff>
--- a/LevelDesign_excel/Level3.xlsx
+++ b/LevelDesign_excel/Level3.xlsx
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y47" sqref="Y47"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF47" sqref="A1:AX51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,8 @@
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="15" width="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="3" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="4" bestFit="1" customWidth="1"/>
     <col min="23" max="48" width="3" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="4" bestFit="1" customWidth="1"/>
@@ -876,8 +877,8 @@
       <c r="AS2" s="13">
         <v>1</v>
       </c>
-      <c r="AT2" s="13">
-        <v>1</v>
+      <c r="AT2" s="16">
+        <v>3</v>
       </c>
       <c r="AU2" s="13">
         <v>1</v>
@@ -1537,8 +1538,8 @@
       <c r="B7" s="13">
         <v>1</v>
       </c>
-      <c r="C7" s="19">
-        <v>33</v>
+      <c r="C7">
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1570,8 +1571,8 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7">
-        <v>0</v>
+      <c r="N7" s="13">
+        <v>1</v>
       </c>
       <c r="O7" s="13">
         <v>1</v>
@@ -1606,8 +1607,8 @@
       <c r="Y7">
         <v>0</v>
       </c>
-      <c r="Z7">
-        <v>0</v>
+      <c r="Z7" s="13">
+        <v>1</v>
       </c>
       <c r="AA7">
         <v>0</v>
@@ -1618,17 +1619,17 @@
       <c r="AC7">
         <v>0</v>
       </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <v>0</v>
-      </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
-      <c r="AG7">
-        <v>0</v>
+      <c r="AD7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="13">
+        <v>1</v>
       </c>
       <c r="AH7">
         <v>0</v>
@@ -1636,14 +1637,14 @@
       <c r="AI7">
         <v>0</v>
       </c>
-      <c r="AJ7">
-        <v>0</v>
+      <c r="AJ7" s="13">
+        <v>1</v>
       </c>
       <c r="AK7">
         <v>0</v>
       </c>
-      <c r="AL7">
-        <v>0</v>
+      <c r="AL7" s="13">
+        <v>1</v>
       </c>
       <c r="AM7">
         <v>0</v>
@@ -1698,29 +1699,29 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13">
+        <v>1</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1728,38 +1729,38 @@
       <c r="M8">
         <v>0</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
+      <c r="N8" s="13">
+        <v>1</v>
+      </c>
+      <c r="O8" s="13">
+        <v>1</v>
       </c>
       <c r="P8" s="13">
         <v>1</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
+      <c r="Q8" s="13">
+        <v>1</v>
+      </c>
+      <c r="R8" s="13">
+        <v>1</v>
+      </c>
+      <c r="S8" s="13">
+        <v>1</v>
+      </c>
+      <c r="T8" s="13">
+        <v>1</v>
+      </c>
+      <c r="U8" s="13">
+        <v>1</v>
       </c>
       <c r="V8">
         <v>0</v>
       </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
+      <c r="W8" s="13">
+        <v>1</v>
+      </c>
+      <c r="X8" s="13">
+        <v>1</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -1770,11 +1771,11 @@
       <c r="AA8">
         <v>0</v>
       </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
+      <c r="AB8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>30</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -1785,11 +1786,11 @@
       <c r="AF8">
         <v>0</v>
       </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
+      <c r="AG8" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="13">
+        <v>1</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -1797,8 +1798,8 @@
       <c r="AJ8">
         <v>0</v>
       </c>
-      <c r="AK8">
-        <v>0</v>
+      <c r="AK8" s="2">
+        <v>30</v>
       </c>
       <c r="AL8">
         <v>0</v>
@@ -1806,8 +1807,8 @@
       <c r="AM8">
         <v>0</v>
       </c>
-      <c r="AN8">
-        <v>0</v>
+      <c r="AN8" s="13">
+        <v>1</v>
       </c>
       <c r="AO8">
         <v>0</v>
@@ -1815,8 +1816,8 @@
       <c r="AP8">
         <v>0</v>
       </c>
-      <c r="AQ8">
-        <v>0</v>
+      <c r="AQ8" s="13">
+        <v>1</v>
       </c>
       <c r="AR8">
         <v>0</v>
@@ -1856,8 +1857,8 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9">
-        <v>0</v>
+      <c r="D9" s="13">
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1877,8 +1878,8 @@
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9">
-        <v>0</v>
+      <c r="K9" s="13">
+        <v>1</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1913,8 +1914,8 @@
       <c r="V9">
         <v>0</v>
       </c>
-      <c r="W9">
-        <v>0</v>
+      <c r="W9" s="13">
+        <v>1</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -1922,53 +1923,53 @@
       <c r="Y9">
         <v>0</v>
       </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <v>0</v>
-      </c>
-      <c r="AD9">
-        <v>0</v>
+      <c r="Z9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="13">
+        <v>1</v>
       </c>
       <c r="AE9">
         <v>0</v>
       </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="2">
-        <v>30</v>
-      </c>
-      <c r="AH9">
-        <v>0</v>
+      <c r="AF9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="13">
+        <v>1</v>
       </c>
       <c r="AI9">
         <v>0</v>
       </c>
-      <c r="AJ9">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="9">
-        <v>14</v>
-      </c>
-      <c r="AL9">
-        <v>0</v>
-      </c>
-      <c r="AM9">
-        <v>0</v>
-      </c>
-      <c r="AN9">
-        <v>0</v>
-      </c>
-      <c r="AO9">
-        <v>0</v>
+      <c r="AJ9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AM9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AN9" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="13">
+        <v>1</v>
       </c>
       <c r="AP9">
         <v>0</v>
@@ -2014,14 +2015,14 @@
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10">
-        <v>0</v>
+      <c r="D10" s="13">
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>0</v>
+      <c r="F10" s="13">
+        <v>1</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -2035,23 +2036,23 @@
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
-        <v>30</v>
+      <c r="K10" s="13">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10">
-        <v>0</v>
+      <c r="N10" s="13">
+        <v>1</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="P10">
-        <v>0</v>
+      <c r="P10" s="18">
+        <v>31</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -2065,35 +2066,35 @@
       <c r="T10">
         <v>0</v>
       </c>
-      <c r="U10">
-        <v>0</v>
+      <c r="U10" s="13">
+        <v>1</v>
       </c>
       <c r="V10">
         <v>0</v>
       </c>
-      <c r="W10">
-        <v>0</v>
+      <c r="W10" s="13">
+        <v>1</v>
       </c>
       <c r="X10">
         <v>0</v>
       </c>
-      <c r="Y10" s="2">
-        <v>30</v>
-      </c>
-      <c r="Z10">
-        <v>0</v>
+      <c r="Y10" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="13">
+        <v>1</v>
       </c>
       <c r="AA10">
         <v>0</v>
       </c>
-      <c r="AB10">
-        <v>0</v>
+      <c r="AB10" s="13">
+        <v>1</v>
       </c>
       <c r="AC10">
         <v>0</v>
       </c>
-      <c r="AD10" s="9">
-        <v>14</v>
+      <c r="AD10">
+        <v>0</v>
       </c>
       <c r="AE10">
         <v>0</v>
@@ -2101,17 +2102,17 @@
       <c r="AF10">
         <v>0</v>
       </c>
-      <c r="AG10">
-        <v>0</v>
-      </c>
-      <c r="AH10">
-        <v>0</v>
+      <c r="AG10" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="13">
+        <v>1</v>
       </c>
       <c r="AI10">
         <v>0</v>
       </c>
-      <c r="AJ10">
-        <v>0</v>
+      <c r="AJ10" s="13">
+        <v>1</v>
       </c>
       <c r="AK10">
         <v>0</v>
@@ -2122,26 +2123,26 @@
       <c r="AM10">
         <v>0</v>
       </c>
-      <c r="AN10">
-        <v>0</v>
-      </c>
-      <c r="AO10">
-        <v>0</v>
-      </c>
-      <c r="AP10">
-        <v>0</v>
+      <c r="AN10" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="13">
+        <v>1</v>
+      </c>
+      <c r="AP10" s="13">
+        <v>1</v>
       </c>
       <c r="AQ10" s="13">
         <v>1</v>
       </c>
-      <c r="AR10">
-        <v>0</v>
-      </c>
-      <c r="AS10">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="9">
-        <v>14</v>
+      <c r="AR10" s="13">
+        <v>1</v>
+      </c>
+      <c r="AS10" s="13">
+        <v>1</v>
+      </c>
+      <c r="AT10" s="13">
+        <v>1</v>
       </c>
       <c r="AU10">
         <v>0</v>
@@ -2166,20 +2167,20 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11">
-        <v>0</v>
+      <c r="D11" s="13">
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>0</v>
+      <c r="F11" s="13">
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>0</v>
+      <c r="H11" s="17">
+        <v>32</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2187,8 +2188,8 @@
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="K11">
-        <v>0</v>
+      <c r="K11" s="13">
+        <v>1</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -2217,14 +2218,14 @@
       <c r="T11">
         <v>0</v>
       </c>
-      <c r="U11">
-        <v>0</v>
+      <c r="U11" s="13">
+        <v>1</v>
       </c>
       <c r="V11">
         <v>0</v>
       </c>
-      <c r="W11">
-        <v>0</v>
+      <c r="W11" s="13">
+        <v>1</v>
       </c>
       <c r="X11">
         <v>0</v>
@@ -2232,29 +2233,29 @@
       <c r="Y11">
         <v>0</v>
       </c>
-      <c r="Z11">
-        <v>0</v>
+      <c r="Z11" s="13">
+        <v>1</v>
       </c>
       <c r="AA11">
         <v>0</v>
       </c>
-      <c r="AB11">
-        <v>0</v>
+      <c r="AB11" s="13">
+        <v>1</v>
       </c>
       <c r="AC11">
         <v>0</v>
       </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
+      <c r="AD11" s="13">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="13">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="13">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="13">
+        <v>1</v>
       </c>
       <c r="AH11">
         <v>0</v>
@@ -2262,20 +2263,20 @@
       <c r="AI11">
         <v>0</v>
       </c>
-      <c r="AJ11">
-        <v>0</v>
+      <c r="AJ11" s="13">
+        <v>1</v>
       </c>
       <c r="AK11">
         <v>0</v>
       </c>
-      <c r="AL11">
-        <v>0</v>
+      <c r="AL11" s="13">
+        <v>1</v>
       </c>
       <c r="AM11">
         <v>0</v>
       </c>
-      <c r="AN11">
-        <v>0</v>
+      <c r="AN11" s="13">
+        <v>1</v>
       </c>
       <c r="AO11">
         <v>0</v>
@@ -2286,8 +2287,8 @@
       <c r="AQ11">
         <v>0</v>
       </c>
-      <c r="AR11">
-        <v>0</v>
+      <c r="AR11" s="18">
+        <v>31</v>
       </c>
       <c r="AS11">
         <v>0</v>
@@ -2330,8 +2331,8 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="F12" s="13">
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -2342,11 +2343,11 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
+      <c r="J12" s="5">
+        <v>13</v>
+      </c>
+      <c r="K12" s="13">
+        <v>1</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -2366,38 +2367,38 @@
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="R12" s="17">
-        <v>32</v>
+      <c r="R12" s="9">
+        <v>14</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12" s="9">
-        <v>14</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
+      <c r="T12" s="13">
+        <v>1</v>
+      </c>
+      <c r="U12" s="13">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12" s="13">
+        <v>1</v>
+      </c>
+      <c r="X12" s="13">
+        <v>1</v>
       </c>
       <c r="Y12">
         <v>0</v>
       </c>
-      <c r="Z12">
-        <v>0</v>
+      <c r="Z12" s="13">
+        <v>1</v>
       </c>
       <c r="AA12">
         <v>0</v>
       </c>
-      <c r="AB12">
-        <v>0</v>
+      <c r="AB12" s="13">
+        <v>1</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -2405,8 +2406,8 @@
       <c r="AD12">
         <v>0</v>
       </c>
-      <c r="AE12">
-        <v>0</v>
+      <c r="AE12" s="13">
+        <v>1</v>
       </c>
       <c r="AF12">
         <v>0</v>
@@ -2417,17 +2418,17 @@
       <c r="AH12" s="9">
         <v>14</v>
       </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-      <c r="AJ12">
-        <v>0</v>
+      <c r="AI12" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="13">
+        <v>1</v>
       </c>
       <c r="AK12">
         <v>0</v>
       </c>
-      <c r="AL12">
-        <v>0</v>
+      <c r="AL12" s="13">
+        <v>1</v>
       </c>
       <c r="AM12">
         <v>0</v>
@@ -2438,23 +2439,23 @@
       <c r="AO12">
         <v>0</v>
       </c>
-      <c r="AP12">
-        <v>0</v>
+      <c r="AP12" s="13">
+        <v>1</v>
       </c>
       <c r="AQ12">
         <v>0</v>
       </c>
-      <c r="AR12">
-        <v>0</v>
-      </c>
-      <c r="AS12">
-        <v>0</v>
+      <c r="AR12" s="13">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="13">
+        <v>1</v>
       </c>
       <c r="AT12">
         <v>0</v>
       </c>
-      <c r="AU12">
-        <v>0</v>
+      <c r="AU12" s="13">
+        <v>1</v>
       </c>
       <c r="AV12">
         <v>0</v>
@@ -2485,11 +2486,11 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="2">
-        <v>30</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -2497,14 +2498,14 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13" s="2">
-        <v>30</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>13</v>
+      </c>
+      <c r="K13" s="13">
+        <v>1</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2533,8 +2534,8 @@
       <c r="T13">
         <v>0</v>
       </c>
-      <c r="U13">
-        <v>0</v>
+      <c r="U13" s="13">
+        <v>1</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -2542,62 +2543,62 @@
       <c r="W13">
         <v>0</v>
       </c>
-      <c r="X13">
-        <v>0</v>
+      <c r="X13" s="13">
+        <v>1</v>
       </c>
       <c r="Y13">
         <v>0</v>
       </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
-      <c r="AB13">
-        <v>0</v>
-      </c>
-      <c r="AC13">
-        <v>0</v>
-      </c>
-      <c r="AD13">
-        <v>0</v>
-      </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
-      <c r="AG13">
-        <v>0</v>
+      <c r="Z13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="18">
+        <v>31</v>
+      </c>
+      <c r="AB13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="5">
+        <v>13</v>
+      </c>
+      <c r="AF13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="13">
+        <v>1</v>
       </c>
       <c r="AH13">
         <v>0</v>
       </c>
-      <c r="AI13">
-        <v>0</v>
-      </c>
-      <c r="AJ13">
-        <v>0</v>
+      <c r="AI13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="13">
+        <v>1</v>
       </c>
       <c r="AK13">
         <v>0</v>
       </c>
-      <c r="AL13" s="9">
-        <v>14</v>
-      </c>
-      <c r="AM13">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="9">
-        <v>14</v>
-      </c>
-      <c r="AO13">
-        <v>0</v>
-      </c>
-      <c r="AP13">
-        <v>0</v>
+      <c r="AL13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AN13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO13" s="13">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="13">
+        <v>1</v>
       </c>
       <c r="AQ13">
         <v>0</v>
@@ -2605,14 +2606,14 @@
       <c r="AR13">
         <v>0</v>
       </c>
-      <c r="AS13">
-        <v>0</v>
+      <c r="AS13" s="13">
+        <v>1</v>
       </c>
       <c r="AT13">
         <v>0</v>
       </c>
-      <c r="AU13">
-        <v>0</v>
+      <c r="AU13" s="13">
+        <v>1</v>
       </c>
       <c r="AV13">
         <v>0</v>
@@ -2640,20 +2641,20 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14">
-        <v>0</v>
+      <c r="D14" s="13">
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14">
-        <v>0</v>
+      <c r="F14" s="13">
+        <v>1</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14">
-        <v>0</v>
+      <c r="H14" s="17">
+        <v>32</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -2661,8 +2662,8 @@
       <c r="J14">
         <v>0</v>
       </c>
-      <c r="K14">
-        <v>0</v>
+      <c r="K14" s="13">
+        <v>1</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2670,14 +2671,14 @@
       <c r="M14">
         <v>0</v>
       </c>
-      <c r="N14">
-        <v>0</v>
+      <c r="N14" s="13">
+        <v>1</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14">
-        <v>0</v>
+      <c r="P14" s="18">
+        <v>31</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -2691,17 +2692,17 @@
       <c r="T14">
         <v>0</v>
       </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
+      <c r="U14" s="13">
+        <v>1</v>
+      </c>
+      <c r="V14" s="13">
+        <v>1</v>
+      </c>
+      <c r="W14" s="13">
+        <v>1</v>
+      </c>
+      <c r="X14" s="13">
+        <v>1</v>
       </c>
       <c r="Y14">
         <v>0</v>
@@ -2712,11 +2713,11 @@
       <c r="AA14">
         <v>0</v>
       </c>
-      <c r="AB14" s="18">
-        <v>31</v>
-      </c>
-      <c r="AC14">
-        <v>0</v>
+      <c r="AB14" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="13">
+        <v>1</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -2733,17 +2734,17 @@
       <c r="AH14">
         <v>0</v>
       </c>
-      <c r="AI14">
-        <v>0</v>
-      </c>
-      <c r="AJ14">
-        <v>0</v>
+      <c r="AI14" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="13">
+        <v>1</v>
       </c>
       <c r="AK14">
         <v>0</v>
       </c>
-      <c r="AL14">
-        <v>0</v>
+      <c r="AL14" s="13">
+        <v>1</v>
       </c>
       <c r="AM14">
         <v>0</v>
@@ -2754,17 +2755,17 @@
       <c r="AO14">
         <v>0</v>
       </c>
-      <c r="AP14">
-        <v>0</v>
+      <c r="AP14" s="13">
+        <v>1</v>
       </c>
       <c r="AQ14">
         <v>0</v>
       </c>
-      <c r="AR14">
-        <v>0</v>
-      </c>
-      <c r="AS14" s="9">
-        <v>14</v>
+      <c r="AR14" s="13">
+        <v>1</v>
+      </c>
+      <c r="AS14" s="13">
+        <v>1</v>
       </c>
       <c r="AT14">
         <v>0</v>
@@ -2798,14 +2799,14 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15">
-        <v>0</v>
+      <c r="D15" s="13">
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15">
-        <v>0</v>
+      <c r="F15" s="13">
+        <v>1</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -2819,8 +2820,8 @@
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15">
-        <v>0</v>
+      <c r="K15" s="13">
+        <v>1</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2855,38 +2856,38 @@
       <c r="V15">
         <v>0</v>
       </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>0</v>
+      <c r="W15" s="13">
+        <v>1</v>
+      </c>
+      <c r="X15" s="13">
+        <v>1</v>
       </c>
       <c r="Y15">
         <v>0</v>
       </c>
-      <c r="Z15">
-        <v>0</v>
+      <c r="Z15" s="13">
+        <v>1</v>
       </c>
       <c r="AA15">
         <v>0</v>
       </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="9">
-        <v>14</v>
+      <c r="AB15" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
       </c>
       <c r="AD15">
         <v>0</v>
       </c>
-      <c r="AE15">
-        <v>0</v>
+      <c r="AE15" s="13">
+        <v>1</v>
       </c>
       <c r="AF15">
         <v>0</v>
       </c>
-      <c r="AG15">
-        <v>0</v>
+      <c r="AG15" s="13">
+        <v>1</v>
       </c>
       <c r="AH15">
         <v>0</v>
@@ -2895,10 +2896,10 @@
         <v>0</v>
       </c>
       <c r="AJ15">
-        <v>0</v>
-      </c>
-      <c r="AK15">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>30</v>
       </c>
       <c r="AL15">
         <v>0</v>
@@ -2906,14 +2907,14 @@
       <c r="AM15">
         <v>0</v>
       </c>
-      <c r="AN15">
-        <v>0</v>
-      </c>
-      <c r="AO15">
-        <v>0</v>
-      </c>
-      <c r="AP15">
-        <v>0</v>
+      <c r="AN15" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO15" s="13">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="13">
+        <v>1</v>
       </c>
       <c r="AQ15">
         <v>0</v>
@@ -2921,17 +2922,17 @@
       <c r="AR15">
         <v>0</v>
       </c>
-      <c r="AS15">
-        <v>0</v>
-      </c>
-      <c r="AT15">
-        <v>0</v>
-      </c>
-      <c r="AU15">
-        <v>0</v>
-      </c>
-      <c r="AV15">
-        <v>0</v>
+      <c r="AS15" s="13">
+        <v>1</v>
+      </c>
+      <c r="AT15" s="13">
+        <v>1</v>
+      </c>
+      <c r="AU15" s="13">
+        <v>1</v>
+      </c>
+      <c r="AV15" s="13">
+        <v>1</v>
       </c>
       <c r="AW15" s="13">
         <v>1</v>
@@ -2956,8 +2957,8 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16">
-        <v>0</v>
+      <c r="D16" s="13">
+        <v>1</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2977,8 +2978,8 @@
       <c r="J16">
         <v>0</v>
       </c>
-      <c r="K16">
-        <v>0</v>
+      <c r="K16" s="13">
+        <v>1</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -2986,35 +2987,35 @@
       <c r="M16">
         <v>0</v>
       </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
+      <c r="N16" s="13">
+        <v>1</v>
+      </c>
+      <c r="O16" s="13">
+        <v>1</v>
       </c>
       <c r="P16" s="13">
         <v>1</v>
       </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
+      <c r="Q16" s="13">
+        <v>1</v>
+      </c>
+      <c r="R16" s="13">
+        <v>1</v>
+      </c>
+      <c r="S16" s="13">
+        <v>1</v>
+      </c>
+      <c r="T16" s="13">
+        <v>1</v>
+      </c>
+      <c r="U16" s="13">
+        <v>1</v>
       </c>
       <c r="V16">
         <v>0</v>
       </c>
-      <c r="W16">
-        <v>0</v>
+      <c r="W16" s="13">
+        <v>1</v>
       </c>
       <c r="X16">
         <v>0</v>
@@ -3025,14 +3026,14 @@
       <c r="Z16">
         <v>0</v>
       </c>
-      <c r="AA16">
-        <v>0</v>
-      </c>
-      <c r="AB16">
-        <v>0</v>
-      </c>
-      <c r="AC16">
-        <v>0</v>
+      <c r="AA16" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="13">
+        <v>1</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -3043,23 +3044,23 @@
       <c r="AF16">
         <v>0</v>
       </c>
-      <c r="AG16">
-        <v>0</v>
-      </c>
-      <c r="AH16">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="9">
-        <v>14</v>
-      </c>
-      <c r="AJ16">
-        <v>0</v>
+      <c r="AG16" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH16" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI16" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="13">
+        <v>1</v>
       </c>
       <c r="AK16">
         <v>0</v>
       </c>
-      <c r="AL16">
-        <v>0</v>
+      <c r="AL16" s="13">
+        <v>1</v>
       </c>
       <c r="AM16">
         <v>0</v>
@@ -3067,8 +3068,8 @@
       <c r="AN16">
         <v>0</v>
       </c>
-      <c r="AO16">
-        <v>0</v>
+      <c r="AO16" s="13">
+        <v>1</v>
       </c>
       <c r="AP16">
         <v>0</v>
@@ -3114,29 +3115,29 @@
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13">
+        <v>1</v>
+      </c>
+      <c r="G17" s="13">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1</v>
+      </c>
+      <c r="I17" s="13">
+        <v>1</v>
+      </c>
+      <c r="J17" s="13">
+        <v>1</v>
+      </c>
+      <c r="K17" s="13">
+        <v>1</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -3144,41 +3145,41 @@
       <c r="M17">
         <v>0</v>
       </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
+      <c r="N17" s="13">
+        <v>1</v>
+      </c>
+      <c r="O17" s="13">
+        <v>1</v>
+      </c>
+      <c r="P17" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="13">
+        <v>1</v>
+      </c>
+      <c r="R17" s="13">
+        <v>1</v>
+      </c>
+      <c r="S17" s="13">
+        <v>1</v>
+      </c>
+      <c r="T17" s="13">
+        <v>1</v>
+      </c>
+      <c r="U17" s="13">
+        <v>1</v>
       </c>
       <c r="V17">
         <v>0</v>
       </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
+      <c r="W17" s="13">
+        <v>1</v>
+      </c>
+      <c r="X17" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="13">
+        <v>1</v>
       </c>
       <c r="Z17">
         <v>0</v>
@@ -3186,8 +3187,8 @@
       <c r="AA17">
         <v>0</v>
       </c>
-      <c r="AB17">
-        <v>0</v>
+      <c r="AB17" s="13">
+        <v>1</v>
       </c>
       <c r="AC17">
         <v>0</v>
@@ -3195,14 +3196,14 @@
       <c r="AD17">
         <v>0</v>
       </c>
-      <c r="AE17">
-        <v>0</v>
+      <c r="AE17" s="13">
+        <v>1</v>
       </c>
       <c r="AF17">
         <v>0</v>
       </c>
-      <c r="AG17">
-        <v>0</v>
+      <c r="AG17" s="13">
+        <v>1</v>
       </c>
       <c r="AH17">
         <v>0</v>
@@ -3216,35 +3217,35 @@
       <c r="AK17">
         <v>0</v>
       </c>
-      <c r="AL17">
-        <v>0</v>
-      </c>
-      <c r="AM17" s="18">
-        <v>31</v>
-      </c>
-      <c r="AN17">
-        <v>0</v>
-      </c>
-      <c r="AO17">
-        <v>0</v>
+      <c r="AL17" s="13">
+        <v>1</v>
+      </c>
+      <c r="AM17" s="13">
+        <v>1</v>
+      </c>
+      <c r="AN17" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO17" s="13">
+        <v>1</v>
       </c>
       <c r="AP17">
         <v>0</v>
       </c>
-      <c r="AQ17">
-        <v>0</v>
-      </c>
-      <c r="AR17" s="9">
-        <v>14</v>
-      </c>
-      <c r="AS17">
-        <v>0</v>
-      </c>
-      <c r="AT17">
-        <v>0</v>
-      </c>
-      <c r="AU17">
-        <v>0</v>
+      <c r="AQ17" s="13">
+        <v>1</v>
+      </c>
+      <c r="AR17" s="13">
+        <v>1</v>
+      </c>
+      <c r="AS17" s="13">
+        <v>1</v>
+      </c>
+      <c r="AT17" s="13">
+        <v>1</v>
+      </c>
+      <c r="AU17" s="13">
+        <v>1</v>
       </c>
       <c r="AV17">
         <v>0</v>
@@ -3278,117 +3279,117 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>0</v>
+      <c r="F18" s="9">
+        <v>14</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9">
+        <v>14</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18" s="13">
+        <v>1</v>
+      </c>
+      <c r="O18" s="13">
+        <v>1</v>
+      </c>
+      <c r="P18" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="13">
+        <v>1</v>
+      </c>
+      <c r="R18" s="13">
+        <v>1</v>
+      </c>
+      <c r="S18" s="13">
+        <v>1</v>
+      </c>
+      <c r="T18" s="13">
+        <v>1</v>
+      </c>
+      <c r="U18" s="13">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="13">
+        <v>1</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="2">
         <v>30</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18" s="13">
-        <v>1</v>
-      </c>
-      <c r="O18" s="13">
-        <v>1</v>
-      </c>
-      <c r="P18" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="13">
-        <v>1</v>
-      </c>
-      <c r="R18" s="13">
-        <v>1</v>
-      </c>
-      <c r="S18" s="13">
-        <v>1</v>
-      </c>
-      <c r="T18" s="13">
-        <v>1</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="9">
-        <v>14</v>
-      </c>
-      <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AA18">
-        <v>0</v>
-      </c>
-      <c r="AB18">
-        <v>0</v>
-      </c>
-      <c r="AC18">
-        <v>0</v>
-      </c>
-      <c r="AD18">
-        <v>0</v>
-      </c>
-      <c r="AE18">
-        <v>0</v>
-      </c>
-      <c r="AF18">
-        <v>0</v>
-      </c>
-      <c r="AG18">
-        <v>0</v>
-      </c>
-      <c r="AH18">
-        <v>0</v>
-      </c>
-      <c r="AI18">
-        <v>0</v>
-      </c>
-      <c r="AJ18">
-        <v>0</v>
-      </c>
-      <c r="AK18">
-        <v>0</v>
-      </c>
-      <c r="AL18">
-        <v>0</v>
-      </c>
-      <c r="AM18">
-        <v>0</v>
-      </c>
-      <c r="AN18">
-        <v>0</v>
-      </c>
-      <c r="AO18">
-        <v>0</v>
-      </c>
-      <c r="AP18">
-        <v>0</v>
-      </c>
       <c r="AQ18">
         <v>0</v>
       </c>
@@ -3401,8 +3402,8 @@
       <c r="AT18">
         <v>0</v>
       </c>
-      <c r="AU18">
-        <v>0</v>
+      <c r="AU18" s="13">
+        <v>1</v>
       </c>
       <c r="AV18">
         <v>0</v>
@@ -3445,8 +3446,8 @@
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19">
-        <v>0</v>
+      <c r="I19" s="9">
+        <v>14</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -3481,14 +3482,14 @@
       <c r="T19" s="13">
         <v>1</v>
       </c>
-      <c r="U19">
-        <v>0</v>
+      <c r="U19" s="13">
+        <v>1</v>
       </c>
       <c r="V19">
         <v>0</v>
       </c>
-      <c r="W19">
-        <v>0</v>
+      <c r="W19" s="13">
+        <v>1</v>
       </c>
       <c r="X19">
         <v>0</v>
@@ -3496,8 +3497,8 @@
       <c r="Y19">
         <v>0</v>
       </c>
-      <c r="Z19">
-        <v>0</v>
+      <c r="Z19" s="13">
+        <v>1</v>
       </c>
       <c r="AA19">
         <v>0</v>
@@ -3505,23 +3506,23 @@
       <c r="AB19">
         <v>0</v>
       </c>
-      <c r="AC19">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="2">
+      <c r="AC19" s="2">
         <v>30</v>
       </c>
-      <c r="AE19">
-        <v>0</v>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="13">
+        <v>1</v>
       </c>
       <c r="AF19">
         <v>0</v>
       </c>
-      <c r="AG19">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="9">
-        <v>14</v>
+      <c r="AG19" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
       </c>
       <c r="AI19">
         <v>0</v>
@@ -3532,35 +3533,35 @@
       <c r="AK19">
         <v>0</v>
       </c>
-      <c r="AL19">
-        <v>0</v>
+      <c r="AL19" s="13">
+        <v>1</v>
       </c>
       <c r="AM19">
         <v>0</v>
       </c>
-      <c r="AN19">
-        <v>0</v>
-      </c>
-      <c r="AO19" s="9">
-        <v>14</v>
+      <c r="AN19" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO19" s="13">
+        <v>1</v>
       </c>
       <c r="AP19">
         <v>0</v>
       </c>
-      <c r="AQ19">
-        <v>0</v>
-      </c>
-      <c r="AR19">
-        <v>0</v>
+      <c r="AQ19" s="13">
+        <v>1</v>
+      </c>
+      <c r="AR19" s="13">
+        <v>1</v>
       </c>
       <c r="AS19">
         <v>0</v>
       </c>
-      <c r="AT19" s="9">
-        <v>14</v>
-      </c>
-      <c r="AU19">
-        <v>0</v>
+      <c r="AT19">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="13">
+        <v>1</v>
       </c>
       <c r="AV19">
         <v>0</v>
@@ -3609,8 +3610,8 @@
       <c r="J20">
         <v>0</v>
       </c>
-      <c r="K20">
-        <v>0</v>
+      <c r="K20" s="19">
+        <v>33</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -3639,65 +3640,65 @@
       <c r="T20" s="13">
         <v>1</v>
       </c>
-      <c r="U20">
-        <v>0</v>
+      <c r="U20" s="13">
+        <v>1</v>
       </c>
       <c r="V20">
         <v>0</v>
       </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="X20">
-        <v>0</v>
+      <c r="W20" s="13">
+        <v>1</v>
+      </c>
+      <c r="X20" s="13">
+        <v>1</v>
       </c>
       <c r="Y20">
         <v>0</v>
       </c>
-      <c r="Z20">
-        <v>0</v>
-      </c>
-      <c r="AA20">
-        <v>0</v>
+      <c r="Z20" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="13">
+        <v>1</v>
       </c>
       <c r="AB20">
         <v>0</v>
       </c>
-      <c r="AC20">
-        <v>0</v>
-      </c>
-      <c r="AD20">
-        <v>0</v>
-      </c>
-      <c r="AE20">
-        <v>0</v>
+      <c r="AC20" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="13">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="13">
+        <v>1</v>
       </c>
       <c r="AF20">
         <v>0</v>
       </c>
-      <c r="AG20">
-        <v>0</v>
+      <c r="AG20" s="13">
+        <v>1</v>
       </c>
       <c r="AH20">
         <v>0</v>
       </c>
-      <c r="AI20">
-        <v>0</v>
-      </c>
-      <c r="AJ20">
-        <v>0</v>
-      </c>
-      <c r="AK20">
-        <v>0</v>
-      </c>
-      <c r="AL20">
-        <v>0</v>
+      <c r="AI20" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ20" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK20" s="13">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="13">
+        <v>1</v>
       </c>
       <c r="AM20">
         <v>0</v>
       </c>
-      <c r="AN20">
-        <v>0</v>
+      <c r="AN20" s="13">
+        <v>1</v>
       </c>
       <c r="AO20">
         <v>0</v>
@@ -3708,17 +3709,17 @@
       <c r="AQ20">
         <v>0</v>
       </c>
-      <c r="AR20">
-        <v>0</v>
+      <c r="AR20" s="13">
+        <v>1</v>
       </c>
       <c r="AS20">
         <v>0</v>
       </c>
-      <c r="AT20">
-        <v>0</v>
-      </c>
-      <c r="AU20">
-        <v>0</v>
+      <c r="AT20" s="13">
+        <v>1</v>
+      </c>
+      <c r="AU20" s="13">
+        <v>1</v>
       </c>
       <c r="AV20">
         <v>0</v>
@@ -3746,14 +3747,14 @@
       <c r="C21" s="13">
         <v>1</v>
       </c>
-      <c r="D21">
-        <v>0</v>
+      <c r="D21" s="13">
+        <v>1</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21">
-        <v>0</v>
+      <c r="F21" s="13">
+        <v>1</v>
       </c>
       <c r="G21" s="13">
         <v>1</v>
@@ -3797,8 +3798,8 @@
       <c r="T21" s="13">
         <v>1</v>
       </c>
-      <c r="U21">
-        <v>0</v>
+      <c r="U21" s="13">
+        <v>1</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -3818,8 +3819,8 @@
       <c r="AA21">
         <v>0</v>
       </c>
-      <c r="AB21">
-        <v>0</v>
+      <c r="AB21" s="9">
+        <v>14</v>
       </c>
       <c r="AC21">
         <v>0</v>
@@ -3830,8 +3831,8 @@
       <c r="AE21">
         <v>0</v>
       </c>
-      <c r="AF21">
-        <v>0</v>
+      <c r="AF21" s="2">
+        <v>30</v>
       </c>
       <c r="AG21">
         <v>0</v>
@@ -3839,8 +3840,8 @@
       <c r="AH21">
         <v>0</v>
       </c>
-      <c r="AI21">
-        <v>0</v>
+      <c r="AI21" s="13">
+        <v>1</v>
       </c>
       <c r="AJ21">
         <v>0</v>
@@ -3854,20 +3855,20 @@
       <c r="AM21">
         <v>0</v>
       </c>
-      <c r="AN21">
-        <v>0</v>
+      <c r="AN21" s="13">
+        <v>1</v>
       </c>
       <c r="AO21">
         <v>0</v>
       </c>
-      <c r="AP21">
-        <v>0</v>
+      <c r="AP21" s="9">
+        <v>14</v>
       </c>
       <c r="AQ21">
         <v>0</v>
       </c>
-      <c r="AR21">
-        <v>0</v>
+      <c r="AR21" s="13">
+        <v>1</v>
       </c>
       <c r="AS21">
         <v>0</v>
@@ -3913,12 +3914,12 @@
       <c r="F22" s="13">
         <v>1</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
+      <c r="G22" s="5">
         <v>13</v>
       </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
       <c r="I22">
         <v>0</v>
       </c>
@@ -3931,8 +3932,8 @@
       <c r="L22">
         <v>0</v>
       </c>
-      <c r="M22" s="13">
-        <v>1</v>
+      <c r="M22">
+        <v>0</v>
       </c>
       <c r="N22" s="13">
         <v>1</v>
@@ -3940,12 +3941,12 @@
       <c r="O22" s="13">
         <v>1</v>
       </c>
-      <c r="P22" s="8">
+      <c r="P22" s="5">
+        <v>13</v>
+      </c>
+      <c r="Q22" s="8">
         <v>121</v>
       </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
       <c r="R22" s="13">
         <v>1</v>
       </c>
@@ -3961,8 +3962,8 @@
       <c r="V22">
         <v>0</v>
       </c>
-      <c r="W22">
-        <v>0</v>
+      <c r="W22" s="18">
+        <v>31</v>
       </c>
       <c r="X22">
         <v>0</v>
@@ -4241,8 +4242,8 @@
       <c r="N24" s="13">
         <v>1</v>
       </c>
-      <c r="O24">
-        <v>0</v>
+      <c r="O24" s="13">
+        <v>1</v>
       </c>
       <c r="P24">
         <v>0</v>
@@ -4364,7 +4365,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="14">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F25" s="13">
         <v>1</v>
@@ -4399,11 +4400,11 @@
       <c r="P25">
         <v>0</v>
       </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="R25">
-        <v>0</v>
+      <c r="Q25" s="17">
+        <v>32</v>
+      </c>
+      <c r="R25" s="13">
+        <v>1</v>
       </c>
       <c r="S25" s="13">
         <v>1</v>
@@ -4527,8 +4528,8 @@
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="I26">
-        <v>0</v>
+      <c r="I26" s="13">
+        <v>1</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -4548,8 +4549,8 @@
       <c r="O26">
         <v>0</v>
       </c>
-      <c r="P26">
-        <v>0</v>
+      <c r="P26" s="13">
+        <v>1</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -4557,8 +4558,8 @@
       <c r="R26">
         <v>0</v>
       </c>
-      <c r="S26" s="19">
-        <v>33</v>
+      <c r="S26">
+        <v>0</v>
       </c>
       <c r="T26" s="13">
         <v>1</v>
@@ -4664,11 +4665,11 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
+      <c r="D27" s="9">
+        <v>14</v>
+      </c>
+      <c r="E27" s="13">
+        <v>1</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -4676,20 +4677,20 @@
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27">
-        <v>0</v>
+      <c r="H27" s="13">
+        <v>1</v>
       </c>
       <c r="I27">
         <v>0</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
         <v>14</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -4819,8 +4820,8 @@
       <c r="D28">
         <v>0</v>
       </c>
-      <c r="E28">
-        <v>0</v>
+      <c r="E28" s="13">
+        <v>1</v>
       </c>
       <c r="F28" s="13">
         <v>1</v>
@@ -4828,20 +4829,20 @@
       <c r="G28">
         <v>0</v>
       </c>
-      <c r="H28">
-        <v>0</v>
+      <c r="H28" s="18">
+        <v>31</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
-      <c r="J28">
-        <v>0</v>
+      <c r="J28" s="13">
+        <v>1</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="L28">
-        <v>0</v>
+      <c r="L28" s="13">
+        <v>1</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -4849,20 +4850,20 @@
       <c r="N28" s="13">
         <v>1</v>
       </c>
-      <c r="O28">
-        <v>0</v>
+      <c r="O28" s="9">
+        <v>14</v>
       </c>
       <c r="P28">
         <v>0</v>
       </c>
-      <c r="Q28">
-        <v>0</v>
+      <c r="Q28" s="13">
+        <v>1</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
-      <c r="S28">
-        <v>0</v>
+      <c r="S28" s="13">
+        <v>1</v>
       </c>
       <c r="T28" s="13">
         <v>1</v>
@@ -4870,26 +4871,26 @@
       <c r="U28">
         <v>0</v>
       </c>
-      <c r="V28">
-        <v>0</v>
-      </c>
-      <c r="W28">
-        <v>0</v>
-      </c>
-      <c r="X28">
-        <v>0</v>
-      </c>
-      <c r="Y28">
-        <v>0</v>
-      </c>
-      <c r="Z28">
-        <v>0</v>
-      </c>
-      <c r="AA28">
-        <v>0</v>
-      </c>
-      <c r="AB28">
-        <v>0</v>
+      <c r="V28" s="13">
+        <v>1</v>
+      </c>
+      <c r="W28" s="13">
+        <v>1</v>
+      </c>
+      <c r="X28" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="13">
+        <v>1</v>
       </c>
       <c r="AC28">
         <v>0</v>
@@ -4912,8 +4913,8 @@
       <c r="AI28">
         <v>0</v>
       </c>
-      <c r="AJ28">
-        <v>0</v>
+      <c r="AJ28" s="13">
+        <v>1</v>
       </c>
       <c r="AK28">
         <v>0</v>
@@ -4948,8 +4949,8 @@
       <c r="AU28">
         <v>0</v>
       </c>
-      <c r="AV28">
-        <v>0</v>
+      <c r="AV28" s="13">
+        <v>1</v>
       </c>
       <c r="AW28" s="13">
         <v>1</v>
@@ -4965,8 +4966,8 @@
       <c r="B29" s="13">
         <v>1</v>
       </c>
-      <c r="C29">
-        <v>0</v>
+      <c r="C29" s="13">
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -4983,8 +4984,8 @@
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="I29">
-        <v>0</v>
+      <c r="I29" s="13">
+        <v>1</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -4992,11 +4993,11 @@
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
+      <c r="L29" s="13">
+        <v>1</v>
+      </c>
+      <c r="M29" s="13">
+        <v>1</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -5037,17 +5038,17 @@
       <c r="Z29">
         <v>0</v>
       </c>
-      <c r="AA29">
-        <v>0</v>
-      </c>
-      <c r="AB29">
-        <v>0</v>
+      <c r="AA29" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="13">
+        <v>1</v>
       </c>
       <c r="AC29">
         <v>0</v>
       </c>
-      <c r="AD29">
-        <v>0</v>
+      <c r="AD29" s="9">
+        <v>14</v>
       </c>
       <c r="AE29">
         <v>0</v>
@@ -5058,50 +5059,50 @@
       <c r="AG29">
         <v>0</v>
       </c>
-      <c r="AH29">
-        <v>0</v>
+      <c r="AH29" s="13">
+        <v>1</v>
       </c>
       <c r="AI29">
         <v>0</v>
       </c>
-      <c r="AJ29">
-        <v>0</v>
+      <c r="AJ29" s="13">
+        <v>1</v>
       </c>
       <c r="AK29">
         <v>0</v>
       </c>
-      <c r="AL29">
-        <v>0</v>
+      <c r="AL29" s="13">
+        <v>1</v>
       </c>
       <c r="AM29">
         <v>0</v>
       </c>
-      <c r="AN29">
-        <v>0</v>
-      </c>
-      <c r="AO29">
-        <v>0</v>
-      </c>
-      <c r="AP29">
-        <v>0</v>
-      </c>
-      <c r="AQ29">
-        <v>0</v>
-      </c>
-      <c r="AR29">
-        <v>0</v>
+      <c r="AN29" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO29" s="13">
+        <v>1</v>
+      </c>
+      <c r="AP29" s="13">
+        <v>1</v>
+      </c>
+      <c r="AQ29" s="13">
+        <v>1</v>
+      </c>
+      <c r="AR29" s="13">
+        <v>1</v>
       </c>
       <c r="AS29">
         <v>0</v>
       </c>
-      <c r="AT29" s="13">
-        <v>1</v>
+      <c r="AT29">
+        <v>0</v>
       </c>
       <c r="AU29">
         <v>0</v>
       </c>
-      <c r="AV29">
-        <v>0</v>
+      <c r="AV29" s="13">
+        <v>1</v>
       </c>
       <c r="AW29" s="13">
         <v>1</v>
@@ -5120,8 +5121,8 @@
       <c r="C30">
         <v>0</v>
       </c>
-      <c r="D30">
-        <v>0</v>
+      <c r="D30" s="13">
+        <v>1</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -5144,8 +5145,8 @@
       <c r="K30">
         <v>0</v>
       </c>
-      <c r="L30" s="9">
-        <v>14</v>
+      <c r="L30">
+        <v>0</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -5156,8 +5157,8 @@
       <c r="O30">
         <v>0</v>
       </c>
-      <c r="P30">
-        <v>0</v>
+      <c r="P30" s="13">
+        <v>1</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -5165,8 +5166,8 @@
       <c r="R30">
         <v>0</v>
       </c>
-      <c r="S30">
-        <v>0</v>
+      <c r="S30" s="13">
+        <v>1</v>
       </c>
       <c r="T30" s="13">
         <v>1</v>
@@ -5174,23 +5175,23 @@
       <c r="U30">
         <v>0</v>
       </c>
-      <c r="V30">
-        <v>0</v>
+      <c r="V30" s="13">
+        <v>1</v>
       </c>
       <c r="W30">
         <v>0</v>
       </c>
-      <c r="X30">
-        <v>0</v>
+      <c r="X30" s="13">
+        <v>1</v>
       </c>
       <c r="Y30">
         <v>0</v>
       </c>
-      <c r="Z30">
-        <v>0</v>
-      </c>
-      <c r="AA30">
-        <v>0</v>
+      <c r="Z30" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="13">
+        <v>1</v>
       </c>
       <c r="AB30">
         <v>0</v>
@@ -5204,26 +5205,26 @@
       <c r="AE30">
         <v>0</v>
       </c>
-      <c r="AF30">
-        <v>0</v>
+      <c r="AF30" s="19">
+        <v>33</v>
       </c>
       <c r="AG30">
         <v>0</v>
       </c>
-      <c r="AH30">
-        <v>0</v>
+      <c r="AH30" s="13">
+        <v>1</v>
       </c>
       <c r="AI30">
         <v>0</v>
       </c>
-      <c r="AJ30">
-        <v>0</v>
-      </c>
-      <c r="AK30" s="18">
-        <v>31</v>
-      </c>
-      <c r="AL30">
-        <v>0</v>
+      <c r="AJ30" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK30">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="13">
+        <v>1</v>
       </c>
       <c r="AM30">
         <v>0</v>
@@ -5234,20 +5235,20 @@
       <c r="AO30">
         <v>0</v>
       </c>
-      <c r="AP30">
-        <v>0</v>
+      <c r="AP30" s="13">
+        <v>1</v>
       </c>
       <c r="AQ30">
         <v>0</v>
       </c>
-      <c r="AR30" s="13">
-        <v>1</v>
+      <c r="AR30">
+        <v>0</v>
       </c>
       <c r="AS30">
         <v>0</v>
       </c>
-      <c r="AT30" s="9">
-        <v>14</v>
+      <c r="AT30" s="13">
+        <v>1</v>
       </c>
       <c r="AU30">
         <v>0</v>
@@ -5323,32 +5324,32 @@
       <c r="T31" s="13">
         <v>1</v>
       </c>
-      <c r="U31">
-        <v>0</v>
-      </c>
-      <c r="V31">
-        <v>0</v>
+      <c r="U31" s="13">
+        <v>1</v>
+      </c>
+      <c r="V31" s="13">
+        <v>1</v>
       </c>
       <c r="W31">
         <v>0</v>
       </c>
-      <c r="X31">
-        <v>0</v>
+      <c r="X31" s="13">
+        <v>1</v>
       </c>
       <c r="Y31">
         <v>0</v>
       </c>
-      <c r="Z31">
-        <v>0</v>
-      </c>
-      <c r="AA31">
-        <v>0</v>
+      <c r="Z31" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="13">
+        <v>1</v>
       </c>
       <c r="AB31">
         <v>0</v>
       </c>
-      <c r="AC31" s="18">
-        <v>31</v>
+      <c r="AC31" s="13">
+        <v>1</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -5362,26 +5363,26 @@
       <c r="AG31">
         <v>0</v>
       </c>
-      <c r="AH31">
-        <v>0</v>
+      <c r="AH31" s="13">
+        <v>1</v>
       </c>
       <c r="AI31">
         <v>0</v>
       </c>
-      <c r="AJ31">
-        <v>0</v>
+      <c r="AJ31" s="13">
+        <v>1</v>
       </c>
       <c r="AK31">
         <v>0</v>
       </c>
-      <c r="AL31">
-        <v>0</v>
+      <c r="AL31" s="13">
+        <v>1</v>
       </c>
       <c r="AM31">
         <v>0</v>
       </c>
-      <c r="AN31">
-        <v>0</v>
+      <c r="AN31" s="13">
+        <v>1</v>
       </c>
       <c r="AO31">
         <v>0</v>
@@ -5389,20 +5390,20 @@
       <c r="AP31" s="13">
         <v>1</v>
       </c>
-      <c r="AQ31" s="9">
-        <v>14</v>
-      </c>
-      <c r="AR31">
-        <v>0</v>
-      </c>
-      <c r="AS31" s="9">
-        <v>14</v>
+      <c r="AQ31">
+        <v>0</v>
+      </c>
+      <c r="AR31" s="13">
+        <v>1</v>
+      </c>
+      <c r="AS31" s="13">
+        <v>1</v>
       </c>
       <c r="AT31" s="13">
         <v>1</v>
       </c>
-      <c r="AU31">
-        <v>0</v>
+      <c r="AU31" s="13">
+        <v>1</v>
       </c>
       <c r="AV31">
         <v>0</v>
@@ -5421,23 +5422,23 @@
       <c r="B32" s="13">
         <v>1</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
+      <c r="C32" s="13">
+        <v>1</v>
+      </c>
+      <c r="D32" s="13">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13">
+        <v>1</v>
+      </c>
+      <c r="F32" s="13">
+        <v>1</v>
+      </c>
+      <c r="G32" s="13">
+        <v>1</v>
+      </c>
+      <c r="H32" s="13">
+        <v>1</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -5448,8 +5449,8 @@
       <c r="K32">
         <v>0</v>
       </c>
-      <c r="L32">
-        <v>0</v>
+      <c r="L32" s="13">
+        <v>1</v>
       </c>
       <c r="M32" s="13">
         <v>1</v>
@@ -5478,35 +5479,35 @@
       <c r="U32">
         <v>0</v>
       </c>
-      <c r="V32">
-        <v>0</v>
+      <c r="V32" s="13">
+        <v>1</v>
       </c>
       <c r="W32">
         <v>0</v>
       </c>
-      <c r="X32">
-        <v>0</v>
+      <c r="X32" s="13">
+        <v>1</v>
       </c>
       <c r="Y32">
         <v>0</v>
       </c>
-      <c r="Z32">
-        <v>0</v>
-      </c>
-      <c r="AA32">
-        <v>0</v>
+      <c r="Z32" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="13">
+        <v>1</v>
       </c>
       <c r="AB32">
         <v>0</v>
       </c>
-      <c r="AC32">
-        <v>0</v>
+      <c r="AC32" s="13">
+        <v>1</v>
       </c>
       <c r="AD32">
         <v>0</v>
       </c>
-      <c r="AE32">
-        <v>0</v>
+      <c r="AE32" s="9">
+        <v>14</v>
       </c>
       <c r="AF32">
         <v>0</v>
@@ -5514,23 +5515,23 @@
       <c r="AG32">
         <v>0</v>
       </c>
-      <c r="AH32">
-        <v>0</v>
-      </c>
-      <c r="AI32">
-        <v>0</v>
-      </c>
-      <c r="AJ32">
-        <v>0</v>
-      </c>
-      <c r="AK32">
-        <v>0</v>
-      </c>
-      <c r="AL32">
-        <v>0</v>
-      </c>
-      <c r="AM32">
-        <v>0</v>
+      <c r="AH32" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI32" s="13">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK32" s="13">
+        <v>1</v>
+      </c>
+      <c r="AL32" s="13">
+        <v>1</v>
+      </c>
+      <c r="AM32" s="2">
+        <v>30</v>
       </c>
       <c r="AN32" s="13">
         <v>1</v>
@@ -5538,23 +5539,23 @@
       <c r="AO32">
         <v>0</v>
       </c>
-      <c r="AP32">
-        <v>0</v>
+      <c r="AP32" s="13">
+        <v>1</v>
       </c>
       <c r="AQ32">
         <v>0</v>
       </c>
-      <c r="AR32" s="13">
-        <v>1</v>
+      <c r="AR32">
+        <v>0</v>
       </c>
       <c r="AS32">
         <v>0</v>
       </c>
-      <c r="AT32" s="9">
-        <v>14</v>
-      </c>
-      <c r="AU32">
-        <v>0</v>
+      <c r="AT32" s="13">
+        <v>1</v>
+      </c>
+      <c r="AU32" s="13">
+        <v>1</v>
       </c>
       <c r="AV32">
         <v>0</v>
@@ -5594,14 +5595,14 @@
       <c r="I33">
         <v>0</v>
       </c>
-      <c r="J33">
-        <v>0</v>
+      <c r="J33" s="13">
+        <v>1</v>
       </c>
       <c r="K33">
         <v>0</v>
       </c>
-      <c r="L33">
-        <v>0</v>
+      <c r="L33" s="13">
+        <v>1</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -5612,8 +5613,8 @@
       <c r="O33">
         <v>0</v>
       </c>
-      <c r="P33">
-        <v>0</v>
+      <c r="P33" s="13">
+        <v>1</v>
       </c>
       <c r="Q33" s="13">
         <v>1</v>
@@ -5630,14 +5631,14 @@
       <c r="U33">
         <v>0</v>
       </c>
-      <c r="V33">
-        <v>0</v>
+      <c r="V33" s="13">
+        <v>1</v>
       </c>
       <c r="W33">
         <v>0</v>
       </c>
-      <c r="X33">
-        <v>0</v>
+      <c r="X33" s="13">
+        <v>1</v>
       </c>
       <c r="Y33">
         <v>0</v>
@@ -5651,8 +5652,8 @@
       <c r="AB33">
         <v>0</v>
       </c>
-      <c r="AC33">
-        <v>0</v>
+      <c r="AC33" s="13">
+        <v>1</v>
       </c>
       <c r="AD33">
         <v>0</v>
@@ -5666,11 +5667,11 @@
       <c r="AG33">
         <v>0</v>
       </c>
-      <c r="AH33">
-        <v>0</v>
-      </c>
-      <c r="AI33">
-        <v>0</v>
+      <c r="AH33" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI33" s="18">
+        <v>31</v>
       </c>
       <c r="AJ33">
         <v>0</v>
@@ -5684,20 +5685,20 @@
       <c r="AM33">
         <v>0</v>
       </c>
-      <c r="AN33">
-        <v>0</v>
-      </c>
-      <c r="AO33">
-        <v>0</v>
+      <c r="AN33" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO33" s="13">
+        <v>1</v>
       </c>
       <c r="AP33" s="13">
         <v>1</v>
       </c>
-      <c r="AQ33">
-        <v>0</v>
-      </c>
-      <c r="AR33">
-        <v>0</v>
+      <c r="AQ33" s="13">
+        <v>1</v>
+      </c>
+      <c r="AR33" s="13">
+        <v>1</v>
       </c>
       <c r="AS33">
         <v>0</v>
@@ -5705,8 +5706,8 @@
       <c r="AT33" s="13">
         <v>1</v>
       </c>
-      <c r="AU33">
-        <v>0</v>
+      <c r="AU33" s="13">
+        <v>1</v>
       </c>
       <c r="AV33">
         <v>0</v>
@@ -5728,44 +5729,44 @@
       <c r="C34">
         <v>0</v>
       </c>
-      <c r="D34">
-        <v>0</v>
+      <c r="D34" s="13">
+        <v>1</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
+      <c r="F34" s="13">
+        <v>1</v>
+      </c>
+      <c r="G34" s="13">
+        <v>1</v>
+      </c>
+      <c r="H34" s="13">
+        <v>1</v>
+      </c>
+      <c r="I34" s="13">
+        <v>1</v>
+      </c>
+      <c r="J34" s="13">
+        <v>1</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
-      <c r="L34">
-        <v>0</v>
+      <c r="L34" s="13">
+        <v>1</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
-      <c r="N34">
-        <v>0</v>
+      <c r="N34" s="13">
+        <v>1</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
-      <c r="P34">
-        <v>0</v>
+      <c r="P34" s="13">
+        <v>1</v>
       </c>
       <c r="Q34">
         <v>0</v>
@@ -5782,32 +5783,32 @@
       <c r="U34">
         <v>0</v>
       </c>
-      <c r="V34">
-        <v>0</v>
+      <c r="V34" s="13">
+        <v>1</v>
       </c>
       <c r="W34">
         <v>0</v>
       </c>
-      <c r="X34">
-        <v>0</v>
-      </c>
-      <c r="Y34">
-        <v>0</v>
-      </c>
-      <c r="Z34">
-        <v>0</v>
-      </c>
-      <c r="AA34">
-        <v>0</v>
-      </c>
-      <c r="AB34">
-        <v>0</v>
-      </c>
-      <c r="AC34">
-        <v>0</v>
-      </c>
-      <c r="AD34">
-        <v>0</v>
+      <c r="X34" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD34" s="13">
+        <v>1</v>
       </c>
       <c r="AE34">
         <v>0</v>
@@ -5818,8 +5819,8 @@
       <c r="AG34">
         <v>0</v>
       </c>
-      <c r="AH34">
-        <v>0</v>
+      <c r="AH34" s="13">
+        <v>1</v>
       </c>
       <c r="AI34">
         <v>0</v>
@@ -5830,8 +5831,8 @@
       <c r="AK34">
         <v>0</v>
       </c>
-      <c r="AL34">
-        <v>0</v>
+      <c r="AL34" s="13">
+        <v>1</v>
       </c>
       <c r="AM34">
         <v>0</v>
@@ -5839,8 +5840,8 @@
       <c r="AN34" s="13">
         <v>1</v>
       </c>
-      <c r="AO34">
-        <v>0</v>
+      <c r="AO34" s="5">
+        <v>13</v>
       </c>
       <c r="AP34">
         <v>0</v>
@@ -5854,8 +5855,8 @@
       <c r="AS34">
         <v>0</v>
       </c>
-      <c r="AT34">
-        <v>0</v>
+      <c r="AT34" s="13">
+        <v>1</v>
       </c>
       <c r="AU34">
         <v>0</v>
@@ -5880,66 +5881,66 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="D35">
-        <v>0</v>
+      <c r="D35" s="13">
+        <v>1</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35" s="2">
+      <c r="F35" s="13">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35" s="13">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35" s="13">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35" s="13">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35" s="13">
+        <v>1</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35" s="13">
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35" s="13">
+        <v>1</v>
+      </c>
+      <c r="W35" s="2">
         <v>30</v>
       </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <v>0</v>
-      </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35">
-        <v>0</v>
-      </c>
-      <c r="S35">
-        <v>0</v>
-      </c>
-      <c r="T35" s="13">
-        <v>1</v>
-      </c>
-      <c r="U35">
-        <v>0</v>
-      </c>
-      <c r="V35">
-        <v>0</v>
-      </c>
-      <c r="W35" s="18">
-        <v>31</v>
-      </c>
       <c r="X35">
         <v>0</v>
       </c>
@@ -5958,11 +5959,11 @@
       <c r="AC35">
         <v>0</v>
       </c>
-      <c r="AD35">
-        <v>0</v>
-      </c>
-      <c r="AE35">
-        <v>0</v>
+      <c r="AD35" s="13">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="13">
+        <v>1</v>
       </c>
       <c r="AF35">
         <v>0</v>
@@ -5973,11 +5974,11 @@
       <c r="AH35" s="13">
         <v>1</v>
       </c>
-      <c r="AI35" s="9">
-        <v>14</v>
-      </c>
-      <c r="AJ35">
-        <v>0</v>
+      <c r="AI35">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="13">
+        <v>1</v>
       </c>
       <c r="AK35">
         <v>0</v>
@@ -5988,11 +5989,11 @@
       <c r="AM35">
         <v>0</v>
       </c>
-      <c r="AN35">
-        <v>0</v>
-      </c>
-      <c r="AO35">
-        <v>0</v>
+      <c r="AN35" s="13">
+        <v>1</v>
+      </c>
+      <c r="AO35" s="13">
+        <v>1</v>
       </c>
       <c r="AP35" s="13">
         <v>1</v>
@@ -6000,8 +6001,8 @@
       <c r="AQ35">
         <v>0</v>
       </c>
-      <c r="AR35">
-        <v>0</v>
+      <c r="AR35" s="13">
+        <v>1</v>
       </c>
       <c r="AS35">
         <v>0</v>
@@ -6012,8 +6013,8 @@
       <c r="AU35">
         <v>0</v>
       </c>
-      <c r="AV35">
-        <v>0</v>
+      <c r="AV35" s="13">
+        <v>1</v>
       </c>
       <c r="AW35" s="13">
         <v>1</v>
@@ -6032,8 +6033,8 @@
       <c r="C36">
         <v>0</v>
       </c>
-      <c r="D36">
-        <v>0</v>
+      <c r="D36" s="13">
+        <v>1</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -6044,14 +6045,14 @@
       <c r="G36">
         <v>0</v>
       </c>
-      <c r="H36">
-        <v>0</v>
+      <c r="H36" s="2">
+        <v>30</v>
       </c>
       <c r="I36">
         <v>0</v>
       </c>
-      <c r="J36">
-        <v>0</v>
+      <c r="J36" s="13">
+        <v>1</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -6062,20 +6063,20 @@
       <c r="M36">
         <v>0</v>
       </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
+      <c r="N36" s="13">
+        <v>1</v>
+      </c>
+      <c r="O36" s="13">
+        <v>1</v>
       </c>
       <c r="P36">
         <v>0</v>
       </c>
-      <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="R36">
-        <v>0</v>
+      <c r="Q36" s="13">
+        <v>1</v>
+      </c>
+      <c r="R36" s="13">
+        <v>1</v>
       </c>
       <c r="S36">
         <v>0</v>
@@ -6086,26 +6087,26 @@
       <c r="U36">
         <v>0</v>
       </c>
-      <c r="V36">
-        <v>0</v>
-      </c>
-      <c r="W36">
-        <v>0</v>
-      </c>
-      <c r="X36">
-        <v>0</v>
-      </c>
-      <c r="Y36">
-        <v>0</v>
-      </c>
-      <c r="Z36">
-        <v>0</v>
+      <c r="V36" s="13">
+        <v>1</v>
+      </c>
+      <c r="W36" s="13">
+        <v>1</v>
+      </c>
+      <c r="X36" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="13">
+        <v>1</v>
       </c>
       <c r="AA36">
         <v>0</v>
       </c>
-      <c r="AB36">
-        <v>0</v>
+      <c r="AB36" s="13">
+        <v>1</v>
       </c>
       <c r="AC36">
         <v>0</v>
@@ -6113,8 +6114,8 @@
       <c r="AD36">
         <v>0</v>
       </c>
-      <c r="AE36">
-        <v>0</v>
+      <c r="AE36" s="13">
+        <v>1</v>
       </c>
       <c r="AF36" s="13">
         <v>1</v>
@@ -6122,8 +6123,8 @@
       <c r="AG36">
         <v>0</v>
       </c>
-      <c r="AH36">
-        <v>0</v>
+      <c r="AH36" s="13">
+        <v>1</v>
       </c>
       <c r="AI36">
         <v>0</v>
@@ -6131,26 +6132,26 @@
       <c r="AJ36" s="13">
         <v>1</v>
       </c>
-      <c r="AK36" s="9">
-        <v>14</v>
-      </c>
-      <c r="AL36">
-        <v>0</v>
+      <c r="AK36">
+        <v>0</v>
+      </c>
+      <c r="AL36" s="13">
+        <v>1</v>
       </c>
       <c r="AM36">
         <v>0</v>
       </c>
-      <c r="AN36" s="13">
-        <v>1</v>
+      <c r="AN36">
+        <v>0</v>
       </c>
       <c r="AO36">
         <v>0</v>
       </c>
-      <c r="AP36">
-        <v>0</v>
-      </c>
-      <c r="AQ36" s="18">
-        <v>31</v>
+      <c r="AP36" s="13">
+        <v>1</v>
+      </c>
+      <c r="AQ36">
+        <v>0</v>
       </c>
       <c r="AR36" s="13">
         <v>1</v>
@@ -6158,8 +6159,8 @@
       <c r="AS36">
         <v>0</v>
       </c>
-      <c r="AT36" s="9">
-        <v>14</v>
+      <c r="AT36" s="13">
+        <v>1</v>
       </c>
       <c r="AU36">
         <v>0</v>
@@ -6184,47 +6185,47 @@
       <c r="C37">
         <v>0</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
+      <c r="D37" s="13">
+        <v>1</v>
+      </c>
+      <c r="E37" s="13">
+        <v>1</v>
+      </c>
+      <c r="F37" s="13">
+        <v>1</v>
+      </c>
+      <c r="G37" s="13">
+        <v>1</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37" s="2">
-        <v>30</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
+      <c r="I37" s="13">
+        <v>1</v>
+      </c>
+      <c r="J37" s="13">
+        <v>1</v>
+      </c>
+      <c r="K37" s="13">
+        <v>1</v>
+      </c>
+      <c r="L37" s="13">
+        <v>1</v>
+      </c>
+      <c r="M37" s="13">
+        <v>1</v>
+      </c>
+      <c r="N37" s="13">
+        <v>1</v>
+      </c>
+      <c r="O37" s="13">
+        <v>1</v>
       </c>
       <c r="P37">
         <v>0</v>
       </c>
-      <c r="Q37">
-        <v>0</v>
+      <c r="Q37" s="13">
+        <v>1</v>
       </c>
       <c r="R37">
         <v>0</v>
@@ -6256,56 +6257,56 @@
       <c r="AA37">
         <v>0</v>
       </c>
-      <c r="AB37">
-        <v>0</v>
-      </c>
-      <c r="AC37">
-        <v>0</v>
-      </c>
-      <c r="AD37" s="13">
-        <v>1</v>
+      <c r="AB37" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC37" s="13">
+        <v>1</v>
+      </c>
+      <c r="AD37">
+        <v>0</v>
       </c>
       <c r="AE37">
         <v>0</v>
       </c>
-      <c r="AF37">
-        <v>0</v>
+      <c r="AF37" s="13">
+        <v>1</v>
       </c>
       <c r="AG37">
         <v>0</v>
       </c>
-      <c r="AH37" s="13">
-        <v>1</v>
+      <c r="AH37">
+        <v>0</v>
       </c>
       <c r="AI37">
         <v>0</v>
       </c>
-      <c r="AJ37">
-        <v>0</v>
+      <c r="AJ37" s="13">
+        <v>1</v>
       </c>
       <c r="AK37">
         <v>0</v>
       </c>
-      <c r="AL37" s="13">
-        <v>1</v>
+      <c r="AL37">
+        <v>0</v>
       </c>
       <c r="AM37">
         <v>0</v>
       </c>
-      <c r="AN37">
-        <v>0</v>
+      <c r="AN37" s="13">
+        <v>1</v>
       </c>
       <c r="AO37">
         <v>0</v>
       </c>
-      <c r="AP37" s="13">
-        <v>1</v>
+      <c r="AP37">
+        <v>0</v>
       </c>
       <c r="AQ37">
         <v>0</v>
       </c>
-      <c r="AR37">
-        <v>0</v>
+      <c r="AR37" s="13">
+        <v>1</v>
       </c>
       <c r="AS37">
         <v>0</v>
@@ -6313,8 +6314,8 @@
       <c r="AT37" s="13">
         <v>1</v>
       </c>
-      <c r="AU37">
-        <v>0</v>
+      <c r="AU37" s="13">
+        <v>1</v>
       </c>
       <c r="AV37">
         <v>0</v>
@@ -6336,8 +6337,8 @@
       <c r="C38">
         <v>0</v>
       </c>
-      <c r="D38" s="2">
-        <v>30</v>
+      <c r="D38">
+        <v>0</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -6345,14 +6346,14 @@
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
+      <c r="G38" s="13">
+        <v>1</v>
+      </c>
+      <c r="H38" s="13">
+        <v>1</v>
+      </c>
+      <c r="I38" s="13">
+        <v>1</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -6363,26 +6364,26 @@
       <c r="L38">
         <v>0</v>
       </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
+      <c r="M38" s="13">
+        <v>1</v>
+      </c>
+      <c r="N38" s="5">
+        <v>13</v>
+      </c>
+      <c r="O38" s="13">
+        <v>1</v>
       </c>
       <c r="P38">
         <v>0</v>
       </c>
-      <c r="Q38">
-        <v>0</v>
+      <c r="Q38" s="13">
+        <v>1</v>
       </c>
       <c r="R38">
         <v>0</v>
       </c>
-      <c r="S38">
-        <v>0</v>
+      <c r="S38" s="13">
+        <v>1</v>
       </c>
       <c r="T38" s="13">
         <v>1</v>
@@ -6491,8 +6492,8 @@
       <c r="D39">
         <v>0</v>
       </c>
-      <c r="E39">
-        <v>0</v>
+      <c r="E39" s="13">
+        <v>1</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -6509,8 +6510,8 @@
       <c r="J39">
         <v>0</v>
       </c>
-      <c r="K39">
-        <v>0</v>
+      <c r="K39" s="13">
+        <v>1</v>
       </c>
       <c r="L39">
         <v>0</v>
@@ -6521,14 +6522,14 @@
       <c r="N39">
         <v>0</v>
       </c>
-      <c r="O39">
-        <v>0</v>
+      <c r="O39" s="13">
+        <v>1</v>
       </c>
       <c r="P39">
         <v>0</v>
       </c>
-      <c r="Q39">
-        <v>0</v>
+      <c r="Q39" s="18">
+        <v>31</v>
       </c>
       <c r="R39">
         <v>0</v>
@@ -7552,8 +7553,8 @@
       <c r="C46">
         <v>0</v>
       </c>
-      <c r="D46" s="9">
-        <v>14</v>
+      <c r="D46">
+        <v>0</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -7567,8 +7568,8 @@
       <c r="H46">
         <v>0</v>
       </c>
-      <c r="I46" s="9">
-        <v>14</v>
+      <c r="I46" s="2">
+        <v>30</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -7582,20 +7583,20 @@
       <c r="M46">
         <v>0</v>
       </c>
-      <c r="N46" s="9">
-        <v>14</v>
-      </c>
-      <c r="O46" s="9">
-        <v>14</v>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
       </c>
       <c r="P46">
         <v>0</v>
       </c>
-      <c r="Q46" s="9">
-        <v>14</v>
-      </c>
-      <c r="R46" s="9">
-        <v>14</v>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
       </c>
       <c r="S46">
         <v>0</v>
@@ -7710,8 +7711,8 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47" s="9">
-        <v>14</v>
+      <c r="F47">
+        <v>0</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -7725,11 +7726,11 @@
       <c r="J47">
         <v>0</v>
       </c>
-      <c r="K47" s="9">
-        <v>14</v>
-      </c>
-      <c r="L47" s="9">
-        <v>14</v>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
       </c>
       <c r="M47">
         <v>0</v>
@@ -7743,8 +7744,8 @@
       <c r="P47">
         <v>0</v>
       </c>
-      <c r="Q47">
-        <v>0</v>
+      <c r="Q47" s="2">
+        <v>30</v>
       </c>
       <c r="R47">
         <v>0</v>

</xml_diff>

<commit_message>
AI teleport bug fixed
</commit_message>
<xml_diff>
--- a/LevelDesign_excel/Level3.xlsx
+++ b/LevelDesign_excel/Level3.xlsx
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF47" sqref="A1:AX51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BC5" sqref="BC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,8 +877,8 @@
       <c r="AS2" s="13">
         <v>1</v>
       </c>
-      <c r="AT2" s="16">
-        <v>3</v>
+      <c r="AT2" s="13">
+        <v>1</v>
       </c>
       <c r="AU2" s="13">
         <v>1</v>
@@ -1035,8 +1035,8 @@
       <c r="AS3" s="13">
         <v>1</v>
       </c>
-      <c r="AT3">
-        <v>0</v>
+      <c r="AT3" s="16">
+        <v>3</v>
       </c>
       <c r="AU3" s="13">
         <v>1</v>
@@ -1193,8 +1193,8 @@
       <c r="AS4" s="13">
         <v>1</v>
       </c>
-      <c r="AT4">
-        <v>0</v>
+      <c r="AT4" s="12">
+        <v>4</v>
       </c>
       <c r="AU4" s="13">
         <v>1</v>
@@ -1351,8 +1351,8 @@
       <c r="AS5" s="13">
         <v>1</v>
       </c>
-      <c r="AT5">
-        <v>0</v>
+      <c r="AT5" s="12">
+        <v>4</v>
       </c>
       <c r="AU5" s="13">
         <v>1</v>
@@ -1509,8 +1509,8 @@
       <c r="AS6" s="13">
         <v>1</v>
       </c>
-      <c r="AT6">
-        <v>0</v>
+      <c r="AT6" s="12">
+        <v>4</v>
       </c>
       <c r="AU6" s="13">
         <v>1</v>

</xml_diff>